<commit_message>
update test files changed name test files(get, create, update, delete)
</commit_message>
<xml_diff>
--- a/Тест-кейсы для api.xlsx
+++ b/Тест-кейсы для api.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="100">
   <si>
     <t>Id</t>
   </si>
@@ -549,16 +549,72 @@
   <si>
     <t>Вопрос аналитику. Требуется ли добавление валидации параметров "name" и "author", должно ли успешно проходить обновление с пустыми значениями.</t>
   </si>
+  <si>
+    <t>Обновить информацию о книге по book_id, отправить запрос  с пустыми параметрами и пустыми значениями</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>1. Отправить запрос
+curl --location --request PUT 'http://192.168.1.64:5000//api/books/2' \
+--header 'Content-Type: application/json' \
+--data-raw '{
+}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Получен код состояния 400 BAD REQUEST
+</t>
+  </si>
+  <si>
+    <t>Удалить  книгу по существующему book_id</t>
+  </si>
+  <si>
+    <t>curl --location --request DELETE 'http://192.168.1.64:5000//api/books/3' \
+--data-raw ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "result": true
+}
+</t>
+  </si>
+  <si>
+    <t>Удалить  книгу по не существующему book_id</t>
+  </si>
+  <si>
+    <t>curl --location --request DELETE 'http://192.168.1.64:5000//api/books/99999999999' \
+--data-raw ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+'error': 'Book with id 99999999999 not found'
+}
+</t>
+  </si>
+  <si>
+    <t>Удалить  книгу по book_id = 0</t>
+  </si>
+  <si>
+    <t>curl --location --request DELETE 'http://192.168.1.64:5000//api/books/0' \
+--data-raw ''</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+'error': 'Book with id 0 not found'
+}
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -585,17 +641,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -613,6 +670,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -621,8 +693,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -636,24 +739,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -667,62 +763,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -737,13 +793,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,169 +961,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,11 +1028,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -998,11 +1084,29 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1021,205 +1125,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1253,14 +1309,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1586,8 +1636,8 @@
   <sheetPr/>
   <dimension ref="A4:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2087,112 +2137,152 @@
       <c r="B30" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+    <row r="31" ht="115.2" spans="1:6">
+      <c r="A31" s="5">
+        <v>27</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" ht="57.6" spans="1:6">
+      <c r="A32" s="5">
+        <v>28</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" ht="57.6" spans="1:6">
+      <c r="A33" s="5">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" ht="57.6" spans="1:6">
+      <c r="A34" s="5">
+        <v>30</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>